<commit_message>
Changement de frmMotDePasse, frmPeriodes
</commit_message>
<xml_diff>
--- a/Journaux de bord/Journal de bord [Antoine].xlsx
+++ b/Journaux de bord/Journal de bord [Antoine].xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Date</t>
   </si>
@@ -44,6 +44,13 @@
 Ajout de code pour confirmer que les boites de textes sont conformes dans frmMain, frmCreation
 Ajout de code dans frmPresence pour empêcher l'utilisateur d'entrer des lettres dans les boites de texte
 Modification complète de frmHoraireSel, l'utilisateur peut seulement sélectionner une période et une journée maintenant </t>
+  </si>
+  <si>
+    <t>lundi 8 février 2016</t>
+  </si>
+  <si>
+    <t>Mise à jour de toutes les formes, elles ne peuvent plus être redimensionnées. 
+Mise à jour de frmMotDePasse, confirmer que le mot de passe est conforme</t>
   </si>
 </sst>
 </file>
@@ -78,7 +85,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -153,11 +160,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -179,6 +195,9 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -483,8 +502,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B1048552"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -525,6 +544,14 @@
         <v>4</v>
       </c>
     </row>
+    <row r="5" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>6</v>
+      </c>
+    </row>
     <row r="1048552" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1048552" s="2"/>
     </row>

</xml_diff>

<commit_message>
Complétion du changement de mot de passe
</commit_message>
<xml_diff>
--- a/Journaux de bord/Journal de bord [Antoine].xlsx
+++ b/Journaux de bord/Journal de bord [Antoine].xlsx
@@ -50,7 +50,7 @@
   </si>
   <si>
     <t>Mise à jour de toutes les formes, elles ne peuvent plus être redimensionnées. 
-Mise à jour de frmMotDePasse, confirmer que le mot de passe est conforme</t>
+Mise à jour de frmMotDePasse, confirmer que le mot de passe est conforme et appel de la procédure stockée pour changer le mot de passe d'un usager (tâche complétée)</t>
   </si>
 </sst>
 </file>
@@ -503,7 +503,7 @@
   <dimension ref="A1:B1048552"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -544,7 +544,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>

</xml_diff>

<commit_message>
Journal de bord (Antoine)
</commit_message>
<xml_diff>
--- a/Journaux de bord/Journal de bord [Antoine].xlsx
+++ b/Journaux de bord/Journal de bord [Antoine].xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Date</t>
   </si>
@@ -51,6 +51,30 @@
   <si>
     <t>Mise à jour de toutes les formes, elles ne peuvent plus être redimensionnées. 
 Mise à jour de frmMotDePasse, confirmer que le mot de passe est conforme</t>
+  </si>
+  <si>
+    <t>mercredi 10 février 2016</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Commencement de l'ajout des périodes requises pour un élève (frmHoraireSel)
+Ajout de toutes les périodes stockées dans la BD sur frmHoraireSel, de façon dynamique.
+</t>
+  </si>
+  <si>
+    <t>lundi 15 février 2016</t>
+  </si>
+  <si>
+    <t>Finalisation de frmHoraireSel: 
+    -Changement des boites à cocher 
+    -Afficher les périodes requises de l'élève sélectionné</t>
+  </si>
+  <si>
+    <t>mercredi 17 février 2016</t>
+  </si>
+  <si>
+    <t>Ajout et finalisation des toutes les fonctionnalités pour les périodes passées et le total des heures (frmCoordonnateur + frmPresences)
+Modification du GUI de frmCoordonnateur
+Ajout du GUI frmPresences</t>
   </si>
 </sst>
 </file>
@@ -85,7 +109,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -94,16 +118,16 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="medium">
+      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -112,68 +136,108 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
       <top/>
-      <bottom/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thick">
         <color indexed="64"/>
       </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top style="thick">
         <color indexed="64"/>
       </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -181,23 +245,35 @@
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -502,8 +578,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B1048552"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -512,32 +588,32 @@
     <col min="2" max="2" width="67.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:2" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="12" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="5">
+    <row r="2" spans="1:2" ht="105.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="9">
         <v>42396</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="10" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="7">
+    <row r="3" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A3" s="3">
         <v>42398</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="7">
+    <row r="4" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A4" s="3">
         <v>42401</v>
       </c>
       <c r="B4" s="4" t="s">
@@ -545,13 +621,38 @@
       </c>
     </row>
     <row r="5" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="6" t="s">
         <v>6</v>
       </c>
     </row>
+    <row r="6" spans="1:2" ht="79.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="1048552" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1048552" s="2"/>
     </row>

</xml_diff>